<commit_message>
fix loc for human_written
</commit_message>
<xml_diff>
--- a/loc_counts.xlsx
+++ b/loc_counts.xlsx
@@ -669,7 +669,7 @@
         <v>7</v>
       </c>
       <c r="C23">
-        <v>23184</v>
+        <v>890</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -680,7 +680,7 @@
         <v>8</v>
       </c>
       <c r="C24">
-        <v>23920</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -691,7 +691,7 @@
         <v>9</v>
       </c>
       <c r="C25">
-        <v>22457</v>
+        <v>163</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -702,7 +702,7 @@
         <v>10</v>
       </c>
       <c r="C26">
-        <v>25595</v>
+        <v>3301</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -713,7 +713,7 @@
         <v>11</v>
       </c>
       <c r="C27">
-        <v>25602</v>
+        <v>3308</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -724,7 +724,7 @@
         <v>12</v>
       </c>
       <c r="C28">
-        <v>22726</v>
+        <v>432</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -735,7 +735,7 @@
         <v>13</v>
       </c>
       <c r="C29">
-        <v>23039</v>
+        <v>745</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add visualizer for the llm responses
</commit_message>
<xml_diff>
--- a/loc_counts.xlsx
+++ b/loc_counts.xlsx
@@ -28,10 +28,10 @@
     <t>c2rust</t>
   </si>
   <si>
-    <t>c2saferust</t>
-  </si>
-  <si>
-    <t>c2saferustv2</t>
+    <t>c2saferrust</t>
+  </si>
+  <si>
+    <t>c2saferrustv2</t>
   </si>
   <si>
     <t>human_written</t>

</xml_diff>